<commit_message>
fix autoselect failure in boundary cell
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="915" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="1365" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>SQ1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,82 @@
   <si>
     <t>ewfwe</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAM1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAM2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAM3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAM4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAM5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARAM6</t>
+  </si>
+  <si>
+    <t>PARAM7</t>
+  </si>
+  <si>
+    <t>PARAM8</t>
+  </si>
+  <si>
+    <t>PARAM9</t>
+  </si>
+  <si>
+    <t>PARAM10</t>
+  </si>
+  <si>
+    <t>PARAM11</t>
+  </si>
+  <si>
+    <t>PARAM12</t>
+  </si>
+  <si>
+    <t>PARAM13</t>
+  </si>
+  <si>
+    <t>PARAM14</t>
+  </si>
+  <si>
+    <t>PARAM15</t>
+  </si>
+  <si>
+    <t>PARAM16</t>
+  </si>
+  <si>
+    <t>PARAM17</t>
   </si>
 </sst>
 </file>
@@ -463,15 +539,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:L19"/>
+  <dimension ref="B4:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -479,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -497,12 +573,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:C11" si="0">VLOOKUP(B6,$H$5:$I$12,2,FALSE)</f>
+        <f t="shared" ref="C6:C10" si="0">VLOOKUP(B6,$H$5:$I$12,2,FALSE)</f>
         <v>CD</v>
       </c>
       <c r="D6" t="s">
@@ -515,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -533,7 +609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -551,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -569,7 +645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -587,7 +663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
         <v>15</v>
       </c>
@@ -595,32 +671,221 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12">
+        <f>1+5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13">
+        <f>88/4</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" t="str">
+        <f>DEC2HEX(200)</f>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="I15">
         <v>1312</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="N15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" t="str">
+        <f>DEC2HEX(53)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="L16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="N17" t="s">
+        <v>34</v>
+      </c>
+      <c r="O17" t="s">
+        <v>31</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" ref="P17" si="1">DEC2HEX(200)</f>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" ref="P18" si="2">DEC2HEX(53)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
         <v>19</v>
+      </c>
+      <c r="N19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" t="s">
+        <v>31</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" ref="P20" si="3">DEC2HEX(200)</f>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>38</v>
+      </c>
+      <c r="O21" t="s">
+        <v>32</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21" si="4">DEC2HEX(53)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>40</v>
+      </c>
+      <c r="O23" t="s">
+        <v>31</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" ref="P23" si="5">DEC2HEX(200)</f>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" t="s">
+        <v>32</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" ref="P24" si="6">DEC2HEX(53)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>42</v>
+      </c>
+      <c r="O25" t="s">
+        <v>33</v>
+      </c>
+      <c r="P25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O26" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26" si="7">DEC2HEX(200)</f>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>44</v>
+      </c>
+      <c r="O27" t="s">
+        <v>32</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" ref="P27" si="8">DEC2HEX(53)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O28" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>